<commit_message>
commit final, trabajo terminado
</commit_message>
<xml_diff>
--- a/proyecto2/Pruebas Proyecto Python - Tienda Virtual.xlsx
+++ b/proyecto2/Pruebas Proyecto Python - Tienda Virtual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODER\proyecto2\proyecto2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97934C0-A3F5-45B2-B9B2-69FE0A1BF992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBCE96C-5229-4CEE-8452-587B0BB9ECC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BCD56C2B-7EFC-4439-B006-08DEE2259B23}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>Nombre del Proyecto</t>
   </si>
@@ -140,9 +140,6 @@
   </si>
   <si>
     <t>Por ahora no hay resultado</t>
-  </si>
-  <si>
-    <t>En lugar de modificar el producto, duplica este mismo.</t>
   </si>
   <si>
     <t>Cuando se edita (boton "editar") la información del producto (ejemplo: camiseta) el usuario es dirigido al detalle del prodcuto, una vez que guarda los cambios, el usuario es redirigido a la lista de productos que se encontraba anteriormente (ejemplo: lista de camisetas)</t>
@@ -171,7 +168,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -234,11 +231,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -557,7 +554,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,65 +571,65 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="5"/>
+      <c r="C1" s="6"/>
       <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="5"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="6">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="5"/>
+      <c r="E2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -658,7 +655,7 @@
       <c r="A7" s="3">
         <v>1</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>45052</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -678,7 +675,7 @@
       <c r="A8" s="3">
         <v>2</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>45052</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -698,7 +695,7 @@
       <c r="A9" s="3">
         <v>3</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>45052</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -718,7 +715,7 @@
       <c r="A10" s="3">
         <v>4</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>45052</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -738,7 +735,7 @@
       <c r="A11" s="3">
         <v>5</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>45052</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -756,35 +753,37 @@
       <c r="A12" s="3">
         <v>6</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>45052</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>7</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>45052</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>16</v>
@@ -794,17 +793,17 @@
       <c r="A14" s="3">
         <v>8</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>45052</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>16</v>
@@ -814,17 +813,17 @@
       <c r="A15" s="3">
         <v>9</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>45052</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>16</v>
@@ -834,17 +833,17 @@
       <c r="A16" s="3">
         <v>10</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>45052</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>16</v>

</xml_diff>